<commit_message>
Structure for producing learning plots
</commit_message>
<xml_diff>
--- a/Parameterization.xlsx
+++ b/Parameterization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Conv Layer</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Signs of overfitting- Training data reach 95% accuracy around epoch 85</t>
+  </si>
+  <si>
+    <t>Orange values may be erroneous</t>
   </si>
 </sst>
 </file>
@@ -64,12 +73,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +414,7 @@
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,8 +439,11 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -437,7 +456,7 @@
       <c r="D2">
         <v>200</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>50</v>
       </c>
       <c r="F2">
@@ -449,8 +468,11 @@
       <c r="I2">
         <v>0.68569999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -463,22 +485,25 @@
       <c r="D3">
         <v>200</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>200</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H3">
-        <v>0.68640000000000001</v>
+        <v>1.4095</v>
       </c>
       <c r="I3">
-        <v>0.71640000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -489,20 +514,20 @@
       <c r="D4">
         <v>200</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>200</v>
       </c>
       <c r="F4">
         <v>20</v>
       </c>
       <c r="H4">
-        <v>0.86670000000000003</v>
+        <v>0.68640000000000001</v>
       </c>
       <c r="I4">
-        <v>0.62070000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.71640000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -515,98 +540,98 @@
       <c r="D5">
         <v>200</v>
       </c>
-      <c r="E5">
-        <v>50</v>
+      <c r="E5" s="1">
+        <v>200</v>
       </c>
       <c r="F5">
         <v>20</v>
       </c>
       <c r="H5">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="I5">
+        <v>0.62070000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="H6">
         <v>0.90849999999999997</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>0.57930000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>100</v>
-      </c>
-      <c r="D6">
-        <v>250</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>1.38</v>
-      </c>
-      <c r="I6">
-        <v>0.43998999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>200</v>
       </c>
       <c r="D7">
         <v>250</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>50</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="H7">
+        <v>1.38</v>
+      </c>
+      <c r="I7">
+        <v>0.43998999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="E8" s="1">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="H8">
         <v>1.18</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>0.54859999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>300</v>
-      </c>
-      <c r="D8">
-        <v>150</v>
-      </c>
-      <c r="E8">
-        <v>200</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>1.0841000000000001</v>
-      </c>
-      <c r="I8">
-        <v>0.58709999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -619,20 +644,20 @@
       <c r="D9">
         <v>150</v>
       </c>
-      <c r="E9">
-        <v>50</v>
+      <c r="E9" s="1">
+        <v>200</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="H9">
-        <v>1.1121000000000001</v>
+        <v>1.0841000000000001</v>
       </c>
       <c r="I9">
-        <v>0.55930000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.58709999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -645,20 +670,20 @@
       <c r="D10">
         <v>150</v>
       </c>
-      <c r="E10">
-        <v>10</v>
+      <c r="E10" s="1">
+        <v>50</v>
       </c>
       <c r="F10">
         <v>5</v>
       </c>
       <c r="H10">
-        <v>1.1060000000000001</v>
+        <v>1.1121000000000001</v>
       </c>
       <c r="I10">
-        <v>0.57930000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.55930000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -671,94 +696,120 @@
       <c r="D11">
         <v>150</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.57930000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="D12">
+        <v>150</v>
+      </c>
+      <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="H11">
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="H12">
         <v>1.1566000000000001</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <v>0.51859999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>300</v>
-      </c>
-      <c r="C12">
-        <v>150</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12">
-        <v>50</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>1.1056999999999999</v>
-      </c>
-      <c r="I12">
-        <v>0.55289999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="C13">
         <v>150</v>
       </c>
       <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>1.1056999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.55289999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
         <v>150</v>
-      </c>
-      <c r="E13">
-        <v>50</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>1.2533000000000001</v>
-      </c>
-      <c r="I13">
-        <v>0.48570000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>200</v>
       </c>
       <c r="C14">
         <v>150</v>
       </c>
       <c r="D14">
+        <v>150</v>
+      </c>
+      <c r="E14" s="1">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>1.2533000000000001</v>
+      </c>
+      <c r="I14">
+        <v>0.48570000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+      <c r="D15">
         <v>100</v>
       </c>
-      <c r="E14">
+      <c r="E15" s="1">
         <v>50</v>
       </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="H14">
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="H15">
         <v>1.2568999999999999</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>0.55069999999999997</v>
       </c>
     </row>

</xml_diff>